<commit_message>
Setando os cenários de login com usuário inválido e usuário vazio.
</commit_message>
<xml_diff>
--- a/Casos de Teste.xlsx
+++ b/Casos de Teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Exercícios Cypress Heroes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932EBC16-7BC7-4940-8E06-33281CC94DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EF953F-5731-4A58-9D2F-EA11697A6487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,14 +19,14 @@
     <sheet name="Status" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Casos de Testes Cypress Heroes'!$A$1:$E$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Casos de Testes Cypress Heroes'!$A$1:$E$40</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
   <si>
     <t>Passos</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Eu como usuário desejo realizar o login com meu e-mail e senha</t>
   </si>
   <si>
-    <t>Inserir um e-mail válido</t>
-  </si>
-  <si>
     <t>Campo disponível para receber as informações do e-mail</t>
   </si>
   <si>
@@ -160,37 +157,94 @@
     <t>Login Admin</t>
   </si>
   <si>
-    <t>Eu como novo usuário desejo me cadastrar no sistema</t>
-  </si>
-  <si>
     <t>Clicar no botão para realizar o login</t>
   </si>
   <si>
-    <t>Clicar no botão cadastrar</t>
-  </si>
-  <si>
     <t>1.4</t>
   </si>
   <si>
     <t>2.4</t>
   </si>
   <si>
-    <t>Botão de cadastro disponível na tela</t>
-  </si>
-  <si>
     <t>3.2</t>
   </si>
   <si>
     <t>3.3</t>
   </si>
   <si>
-    <t>Inserir uma senha válida</t>
-  </si>
-  <si>
     <t>3.4</t>
   </si>
   <si>
-    <t>Clicar no botão para submeter o cadastro</t>
+    <t>Login Inválido</t>
+  </si>
+  <si>
+    <t>Eu como novo usuário desejo realizar o login com uma conta não cadastrada</t>
+  </si>
+  <si>
+    <t>Inserir um e-mail não cadastrado</t>
+  </si>
+  <si>
+    <t>Inserir a senha não cadastrada</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>Mensagem de logado com sucesso</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>Mensagem de email ou senha inválida</t>
+  </si>
+  <si>
+    <t>Login em branco</t>
+  </si>
+  <si>
+    <t>Eu como usuário desejo realizar o login sem inserir email e senha</t>
+  </si>
+  <si>
+    <t>Não é exiibida nenhuma informação de logado com sucesso ou boas vindas</t>
+  </si>
+  <si>
+    <t>Campo informando que nescessita de um e-mail válido</t>
+  </si>
+  <si>
+    <t>Campo informando que nescessita de uma senha válida</t>
+  </si>
+  <si>
+    <t>Exibida a mensagem de usuário ou senha inválido</t>
+  </si>
+  <si>
+    <t>Usuário logado</t>
+  </si>
+  <si>
+    <t>Exibir mensagem de erro</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>Deixar o campo de e-mail em branco</t>
+  </si>
+  <si>
+    <t>Deixar o campo de senha em branco</t>
+  </si>
+  <si>
+    <t>Não é exibida mensagem de logar com usuário ou senha em branco</t>
   </si>
 </sst>
 </file>
@@ -200,7 +254,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\.m"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -268,13 +322,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -326,7 +373,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -514,6 +561,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -586,21 +642,53 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="2"/>
@@ -742,14 +830,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="Casos de Testes Cadastro-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="17"/>
+      <tableStyleElement type="firstRowStripe" dxfId="16"/>
+      <tableStyleElement type="secondRowStripe" dxfId="15"/>
+    </tableStyle>
+    <tableStyle name="Casos de Testes Login-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="14"/>
       <tableStyleElement type="firstRowStripe" dxfId="13"/>
       <tableStyleElement type="secondRowStripe" dxfId="12"/>
-    </tableStyle>
-    <tableStyle name="Casos de Testes Login-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="11"/>
-      <tableStyleElement type="firstRowStripe" dxfId="10"/>
-      <tableStyleElement type="secondRowStripe" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -764,8 +852,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Casos_de_Testes_de_Cdastro" displayName="Casos_de_Testes_de_Cdastro" ref="A1:E36">
-  <autoFilter ref="A1:E36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Casos_de_Testes_de_Cdastro" displayName="Casos_de_Testes_de_Cdastro" ref="A1:E40">
+  <autoFilter ref="A1:E40" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarefa"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Passos"/>
@@ -978,19 +1066,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5703125" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -1026,10 +1114,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>19</v>
@@ -1037,258 +1125,340 @@
     </row>
     <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
-        <v>36</v>
+      <c r="A5" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
-        <v>47</v>
+      <c r="A6" s="26" t="s">
+        <v>44</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="20">
+        <v>2</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="20">
-        <v>2</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>34</v>
+      <c r="A10" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>38</v>
+      <c r="A11" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
+    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="20">
-        <v>3</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>49</v>
+      <c r="A13" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="20">
+        <v>3</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
       <c r="D18" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="20">
+        <v>4</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="D27" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="D19" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="5"/>
-      <c r="D20" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="D23" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="5"/>
-      <c r="D24" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="D25" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
@@ -1307,68 +1477,157 @@
     <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="5" t="s">
+    <row r="31" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="5"/>
+      <c r="D32" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="D33" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="5"/>
       <c r="D34" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
       <c r="D35" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="5" t="s">
+    <row r="36" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+      <c r="D37" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="5"/>
+      <c r="D38" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="D39" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="9"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="5" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"Bloqueado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D11 D3:D6">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
+  <conditionalFormatting sqref="D3:D7 D9:D13">
+    <cfRule type="cellIs" dxfId="8" priority="22" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:D19">
+    <cfRule type="cellIs" dxfId="7" priority="20" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:D30">
+    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32:D35">
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="15">
@@ -1382,8 +1641,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D16">
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
+  <conditionalFormatting sqref="D37:D40">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="13">
@@ -1397,11 +1656,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18:D21">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+  <conditionalFormatting sqref="D21:D25">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1412,41 +1671,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D23:D26">
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+  <conditionalFormatting sqref="D25">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D31">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
-      <formula>"Pronto"</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33:D36">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>"Pronto"</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1458,7 +1687,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D28:D31 D13:D16 D18:D21 D23:D26 D33:D36 D3:D11" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D32:D35 D27:D30 D37:D40 D3:D13 D15:D19 D21:D25" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Pronto,Passou,Bloqueado,Falhou"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Configurando a classe e o spec de interação com usuario logado.
</commit_message>
<xml_diff>
--- a/Casos de Teste.xlsx
+++ b/Casos de Teste.xlsx
@@ -8,25 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Exercícios Cypress Heroes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EF953F-5731-4A58-9D2F-EA11697A6487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0EA45E-F9E6-4BEC-A7B8-AB82908F8EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Casos de Testes Cypress Heroes" sheetId="1" r:id="rId1"/>
-    <sheet name="Modelo de Casos de Teste Login" sheetId="3" r:id="rId2"/>
-    <sheet name="Modelo de Casos de Teste Cadast" sheetId="4" r:id="rId3"/>
-    <sheet name="Status" sheetId="5" r:id="rId4"/>
+    <sheet name="Casos de Testes Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Casos de Testes Interação" sheetId="6" r:id="rId2"/>
+    <sheet name="Modelo de Casos de Teste Login" sheetId="3" r:id="rId3"/>
+    <sheet name="Modelo de Casos de Teste Cadast" sheetId="4" r:id="rId4"/>
+    <sheet name="Status" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Casos de Testes Cypress Heroes'!$A$1:$E$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Casos de Testes Interação'!$A$1:$E$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Casos de Testes Login'!$A$1:$E$40</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="91">
   <si>
     <t>Passos</t>
   </si>
@@ -245,6 +247,60 @@
   </si>
   <si>
     <t>Não é exibida mensagem de logar com usuário ou senha em branco</t>
+  </si>
+  <si>
+    <t>Login Sucesso</t>
+  </si>
+  <si>
+    <t>Curtir o Heroi</t>
+  </si>
+  <si>
+    <t>Eu como usuário logado quero curtir o meu herói favorito</t>
+  </si>
+  <si>
+    <t>Clicar no ícone / botão de curtir</t>
+  </si>
+  <si>
+    <t>Contratar o Heroi</t>
+  </si>
+  <si>
+    <t>Eu como usuário logado quero contratar um herói</t>
+  </si>
+  <si>
+    <t>Clicar no ícone / botão de contratar</t>
+  </si>
+  <si>
+    <t>Botão disponível, acrescenta em um a informação de fans após a interação</t>
+  </si>
+  <si>
+    <t>Botão disponível, acrescenta em um a informação de save após a interação</t>
+  </si>
+  <si>
+    <t>Acrescentou em um a informação de fans após a interação com o botão curtir</t>
+  </si>
+  <si>
+    <t>Acrescentou em um a informação de fans após a interação com o botão contratar</t>
+  </si>
+  <si>
+    <t>Desistir da Contratação</t>
+  </si>
+  <si>
+    <t>Eu como usuário logado quero desistir na confirmação de contratar um herói</t>
+  </si>
+  <si>
+    <t>Clicar no botão para confirmar a contratação</t>
+  </si>
+  <si>
+    <t>Botão disponível, exibe um modal com a confirmação ou não da contratação</t>
+  </si>
+  <si>
+    <t>Modal exibido com as infomações de confirmar ou desistir da contratação</t>
+  </si>
+  <si>
+    <t>Clicar no botão para cancelar a contratação</t>
+  </si>
+  <si>
+    <t>Operação de contratação cancelada</t>
   </si>
 </sst>
 </file>
@@ -658,7 +714,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="30">
     <dxf>
       <font>
         <color theme="2"/>
@@ -755,7 +811,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
+          <bgColor rgb="FF002060"/>
         </patternFill>
       </fill>
     </dxf>
@@ -765,7 +821,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEE0000"/>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -775,6 +831,126 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFEE0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="1" tint="0.34998626667073579"/>
         </patternFill>
       </fill>
@@ -830,14 +1006,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="Casos de Testes Cadastro-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="17"/>
-      <tableStyleElement type="firstRowStripe" dxfId="16"/>
-      <tableStyleElement type="secondRowStripe" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="29"/>
+      <tableStyleElement type="firstRowStripe" dxfId="28"/>
+      <tableStyleElement type="secondRowStripe" dxfId="27"/>
     </tableStyle>
     <tableStyle name="Casos de Testes Login-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="firstRowStripe" dxfId="13"/>
-      <tableStyleElement type="secondRowStripe" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+      <tableStyleElement type="firstRowStripe" dxfId="25"/>
+      <tableStyleElement type="secondRowStripe" dxfId="24"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -860,6 +1036,20 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Resultado Esperado"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Status"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Resultados Encontrados"/>
+  </tableColumns>
+  <tableStyleInfo name="Casos de Testes Cadastro-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{322BFF2D-F3C5-4B2F-82BB-31FFFAA6DC8A}" name="Casos_de_Testes_de_Cdastro3" displayName="Casos_de_Testes_de_Cdastro3" ref="A1:E40">
+  <autoFilter ref="A1:E40" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B764DFCB-40D1-4635-B307-92EAE47FD389}" name="Tarefa"/>
+    <tableColumn id="2" xr3:uid="{881FC81E-03FC-44CB-9EA6-8BC8D536F78B}" name="Passos"/>
+    <tableColumn id="3" xr3:uid="{FA455515-3A07-440F-A015-8EFEBEC2E935}" name="Resultado Esperado"/>
+    <tableColumn id="4" xr3:uid="{59086E64-B159-49D5-88FE-724A5F64C2BD}" name="Status"/>
+    <tableColumn id="5" xr3:uid="{286E11D1-6CC8-47F2-B446-C1945F80D859}" name="Resultados Encontrados"/>
   </tableColumns>
   <tableStyleInfo name="Casos de Testes Cadastro-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1068,9 +1258,9 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1100,7 +1290,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>29</v>
@@ -1556,18 +1746,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>"Bloqueado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D7 D9:D13">
-    <cfRule type="cellIs" dxfId="8" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="23">
@@ -1582,7 +1772,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D19">
-    <cfRule type="cellIs" dxfId="7" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="21">
@@ -1597,7 +1787,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -1611,8 +1801,38 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D25">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D27:D30">
-    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="17">
@@ -1627,7 +1847,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D35">
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="15">
@@ -1642,40 +1862,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D40">
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21:D25">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"Pronto"</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Pronto"</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1699,6 +1889,555 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A6D74A-1D47-429A-A298-26BB8DEC8664}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="20">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="23"/>
+      <c r="B4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="25"/>
+      <c r="B5" s="7"/>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="26"/>
+      <c r="B6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="27"/>
+      <c r="B7" s="28"/>
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="20">
+        <v>2</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="25"/>
+      <c r="B11" s="7"/>
+      <c r="D11" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="26"/>
+      <c r="B12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="27"/>
+      <c r="B13" s="28"/>
+      <c r="D13" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="20">
+        <v>3</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="25"/>
+      <c r="B17" s="7"/>
+      <c r="D17" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="26"/>
+      <c r="B18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="27"/>
+      <c r="B19" s="28"/>
+      <c r="D19" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="24"/>
+      <c r="D21" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="23"/>
+      <c r="B22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="25"/>
+      <c r="B23" s="7"/>
+      <c r="D23" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="26"/>
+      <c r="B24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
+      <c r="D25" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="D27" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="D29" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="D33" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="5"/>
+      <c r="D34" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+      <c r="D37" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="5"/>
+      <c r="D38" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="D39" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="9"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+      <formula>"Bloqueado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>"Falhou"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+      <formula>"Passou"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D7 D9:D13">
+    <cfRule type="cellIs" dxfId="9" priority="22" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:D19">
+    <cfRule type="cellIs" dxfId="8" priority="20" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D25">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:D30">
+    <cfRule type="cellIs" dxfId="4" priority="18" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32:D35">
+    <cfRule type="cellIs" dxfId="3" priority="16" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37:D40">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:D19">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D25">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D32:D35 D27:D30 D37:D40 D15:D19 D3:D13 D21:D25" xr:uid="{051BBB70-4ED9-4C16-9CA7-799D302B925B}">
+      <formula1>"Pronto,Passou,Bloqueado,Falhou"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1784,7 +2523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1868,7 +2607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
Criando a classe de criação do novo heroi.
</commit_message>
<xml_diff>
--- a/Casos de Teste.xlsx
+++ b/Casos de Teste.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Exercícios Cypress Heroes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0EA45E-F9E6-4BEC-A7B8-AB82908F8EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6457085-3BF3-4643-9BEE-2E37D4C43EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Testes Login" sheetId="1" r:id="rId1"/>
     <sheet name="Casos de Testes Interação" sheetId="6" r:id="rId2"/>
-    <sheet name="Modelo de Casos de Teste Login" sheetId="3" r:id="rId3"/>
-    <sheet name="Modelo de Casos de Teste Cadast" sheetId="4" r:id="rId4"/>
-    <sheet name="Status" sheetId="5" r:id="rId5"/>
+    <sheet name="Casos de Testes Ações Admin" sheetId="7" r:id="rId3"/>
+    <sheet name="Modelo de Casos de Teste Login" sheetId="3" r:id="rId4"/>
+    <sheet name="Modelo de Casos de Teste Cadast" sheetId="4" r:id="rId5"/>
+    <sheet name="Status" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Casos de Testes Ações Admin'!$A$1:$E$43</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Casos de Testes Interação'!$A$1:$E$40</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Casos de Testes Login'!$A$1:$E$40</definedName>
   </definedNames>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="111">
   <si>
     <t>Passos</t>
   </si>
@@ -301,6 +303,66 @@
   </si>
   <si>
     <t>Operação de contratação cancelada</t>
+  </si>
+  <si>
+    <t>Criar novo Heroi</t>
+  </si>
+  <si>
+    <t>Eu como usuário administrador logado, desejo criar um novo heroi</t>
+  </si>
+  <si>
+    <t>Clicar no botão para criar um novo heroi</t>
+  </si>
+  <si>
+    <t>Botão disponível na tela do admin</t>
+  </si>
+  <si>
+    <t>Botão para criar novo heroi disponível na tela do admin</t>
+  </si>
+  <si>
+    <t>Inserir um nome para o heroi</t>
+  </si>
+  <si>
+    <t>Inserir um preço para o heroi</t>
+  </si>
+  <si>
+    <t>Inserir a quantidade de curtidas iniciais do heroi</t>
+  </si>
+  <si>
+    <t>Inserir a quantidade incial de contratações do heroi</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>Escolher o poder do heroi</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>Escolher o avatar do heroi</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>Clicar no botão para submeter o cadastro e criar o novo heroi</t>
+  </si>
+  <si>
+    <t>Campo pronto para receber a informação alfanumérica</t>
+  </si>
+  <si>
+    <t>Campo pronto para receber a informação numérica</t>
+  </si>
+  <si>
+    <t>Campo de multipla escolha disponível</t>
+  </si>
+  <si>
+    <t>Opção para enviar o avatar do meu computador</t>
+  </si>
+  <si>
+    <t>Botão de submeter disponpivel na tela</t>
   </si>
 </sst>
 </file>
@@ -630,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -710,11 +772,164 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="2"/>
@@ -1006,14 +1221,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="Casos de Testes Cadastro-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="29"/>
-      <tableStyleElement type="firstRowStripe" dxfId="28"/>
-      <tableStyleElement type="secondRowStripe" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="44"/>
+      <tableStyleElement type="firstRowStripe" dxfId="43"/>
+      <tableStyleElement type="secondRowStripe" dxfId="42"/>
     </tableStyle>
     <tableStyle name="Casos de Testes Login-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="26"/>
-      <tableStyleElement type="firstRowStripe" dxfId="25"/>
-      <tableStyleElement type="secondRowStripe" dxfId="24"/>
+      <tableStyleElement type="headerRow" dxfId="41"/>
+      <tableStyleElement type="firstRowStripe" dxfId="40"/>
+      <tableStyleElement type="secondRowStripe" dxfId="39"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1050,6 +1265,20 @@
     <tableColumn id="3" xr3:uid="{FA455515-3A07-440F-A015-8EFEBEC2E935}" name="Resultado Esperado"/>
     <tableColumn id="4" xr3:uid="{59086E64-B159-49D5-88FE-724A5F64C2BD}" name="Status"/>
     <tableColumn id="5" xr3:uid="{286E11D1-6CC8-47F2-B446-C1945F80D859}" name="Resultados Encontrados"/>
+  </tableColumns>
+  <tableStyleInfo name="Casos de Testes Cadastro-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BC73408C-81A1-48D1-8F13-6717416C4DE9}" name="Casos_de_Testes_de_Cdastro4" displayName="Casos_de_Testes_de_Cdastro4" ref="A1:E43">
+  <autoFilter ref="A1:E43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{1D37A878-E798-421B-A727-C232DAE7ADF1}" name="Tarefa"/>
+    <tableColumn id="2" xr3:uid="{357F3411-C044-4F9D-8E9A-D912BA9EC96D}" name="Passos"/>
+    <tableColumn id="3" xr3:uid="{89543A9C-6885-4218-8097-A7EEFD9B17C2}" name="Resultado Esperado"/>
+    <tableColumn id="4" xr3:uid="{24EEFF8E-DA59-46E1-B46B-CD66E3C2FCD0}" name="Status"/>
+    <tableColumn id="5" xr3:uid="{E3E4649C-C521-43C8-9BB9-C9BB6C5E3698}" name="Resultados Encontrados"/>
   </tableColumns>
   <tableStyleInfo name="Casos de Testes Cadastro-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1259,7 +1488,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1746,18 +1975,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
       <formula>"Bloqueado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="11" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D7 D9:D13">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="22" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="23">
@@ -1772,7 +2001,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D19">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="20" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="21">
@@ -1787,7 +2016,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -1802,7 +2031,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D25">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -1817,7 +2046,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -1832,7 +2061,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D30">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="17">
@@ -1847,7 +2076,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D35">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="14" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="15">
@@ -1862,7 +2091,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D40">
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="13">
@@ -1895,9 +2124,9 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2265,18 +2494,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
       <formula>"Bloqueado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D7 D9:D13">
-    <cfRule type="cellIs" dxfId="9" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="23">
@@ -2291,7 +2520,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D19">
-    <cfRule type="cellIs" dxfId="8" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="21">
@@ -2306,7 +2548,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
@@ -2321,7 +2563,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D25">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="8">
@@ -2336,7 +2591,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -2351,7 +2606,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D30">
-    <cfRule type="cellIs" dxfId="4" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="19">
@@ -2366,7 +2621,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D35">
-    <cfRule type="cellIs" dxfId="3" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="17">
@@ -2381,40 +2636,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D40">
-    <cfRule type="cellIs" dxfId="2" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15:D19">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"Pronto"</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21:D25">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Pronto"</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2438,6 +2663,607 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CBC95CF-1C12-4AB7-99DA-4D4D10D459B3}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:E43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" customWidth="1"/>
+    <col min="5" max="5" width="65.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="20">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="21"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
+      <c r="B12" s="24"/>
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="23"/>
+      <c r="B13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="25"/>
+      <c r="B14" s="7"/>
+      <c r="D14" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="26"/>
+      <c r="B15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="D16" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="24"/>
+      <c r="D18" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="23"/>
+      <c r="B19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="25"/>
+      <c r="B20" s="7"/>
+      <c r="D20" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="26"/>
+      <c r="B21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="27"/>
+      <c r="B22" s="28"/>
+      <c r="D22" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="20"/>
+      <c r="B24" s="24"/>
+      <c r="D24" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="23"/>
+      <c r="B25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="25"/>
+      <c r="B26" s="7"/>
+      <c r="D26" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="26"/>
+      <c r="B27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="27"/>
+      <c r="B28" s="28"/>
+      <c r="D28" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="D30" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="D32" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+      <c r="B35" s="5"/>
+      <c r="D35" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="D36" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="5"/>
+      <c r="D37" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="D40" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="5"/>
+      <c r="D41" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="D42" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="9"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+      <formula>"Bloqueado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
+      <formula>"Falhou"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
+      <formula>"Passou"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D16 D3:D10">
+    <cfRule type="cellIs" dxfId="11" priority="26" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:D22">
+    <cfRule type="cellIs" dxfId="10" priority="24" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24:D28">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30:D33">
+    <cfRule type="cellIs" dxfId="6" priority="22" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35:D38">
+    <cfRule type="cellIs" dxfId="5" priority="20" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:D43">
+    <cfRule type="cellIs" dxfId="4" priority="18" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24:D28">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:D22 D12:D16 D3:D10">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10 D22 D16">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:D22">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D35:D38 D30:D33 D40:D43 D24:D28 D18:D22 D3:D16" xr:uid="{114A343E-435B-4E65-82C9-A3F3E795374C}">
+      <formula1>"Pronto,Passou,Bloqueado,Falhou"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2523,7 +3349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2607,7 +3433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
Finalizado o teste de editar um heroi.
</commit_message>
<xml_diff>
--- a/Casos de Teste.xlsx
+++ b/Casos de Teste.xlsx
@@ -8,20 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Exercícios Cypress Heroes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6457085-3BF3-4643-9BEE-2E37D4C43EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83FFD76-51D4-4C95-AB05-8F404CF590DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Testes Login" sheetId="1" r:id="rId1"/>
     <sheet name="Casos de Testes Interação" sheetId="6" r:id="rId2"/>
     <sheet name="Casos de Testes Ações Admin" sheetId="7" r:id="rId3"/>
-    <sheet name="Modelo de Casos de Teste Login" sheetId="3" r:id="rId4"/>
-    <sheet name="Modelo de Casos de Teste Cadast" sheetId="4" r:id="rId5"/>
-    <sheet name="Status" sheetId="5" r:id="rId6"/>
+    <sheet name="Status" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Casos de Testes Ações Admin'!$A$1:$E$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Casos de Testes Ações Admin'!$A$1:$E$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Casos de Testes Interação'!$A$1:$E$40</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Casos de Testes Login'!$A$1:$E$40</definedName>
   </definedNames>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="119">
   <si>
     <t>Passos</t>
   </si>
@@ -44,69 +42,12 @@
     <t>Resultados Encontrados</t>
   </si>
   <si>
-    <t>Précondições</t>
-  </si>
-  <si>
     <t>Pronto</t>
   </si>
   <si>
-    <t>Título</t>
-  </si>
-  <si>
-    <t>Logando com e-mail e senha válidos</t>
-  </si>
-  <si>
-    <t>Usuário previamente cadastrado no sistema</t>
-  </si>
-  <si>
-    <t>Passo a passo</t>
-  </si>
-  <si>
-    <t>Inserir e-mail cadastrado / inserir a senha cadastrada / clicar no botão login</t>
-  </si>
-  <si>
-    <t>Resultado esperado</t>
-  </si>
-  <si>
-    <t>Usuário loga com sucesso / usuário é redirecionado para a página inicial</t>
-  </si>
-  <si>
-    <t>Suite de teste</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Ambiente de teste</t>
-  </si>
-  <si>
-    <t>Navegador Google Chrome Versão 135.0.7049.96 / Windows 11 64 bits</t>
-  </si>
-  <si>
-    <t>Resultado encontrado</t>
-  </si>
-  <si>
-    <t>O mesmo do resultado esperado</t>
-  </si>
-  <si>
     <t>Passou</t>
   </si>
   <si>
-    <t>Cadastrando um usuário com dados os válidos</t>
-  </si>
-  <si>
-    <t>Não possui</t>
-  </si>
-  <si>
-    <t>Inserir o nome do usuário / inserir um e-mail válido / inserir a senha  / clicar no botão cadastrar</t>
-  </si>
-  <si>
-    <t>Sistema exibe a mensagemd e usuário cadastrado com sucesso / usuário é redirecionado para a página principal</t>
-  </si>
-  <si>
-    <t>Cadastro</t>
-  </si>
-  <si>
     <t>Status dos Testes</t>
   </si>
   <si>
@@ -363,6 +304,87 @@
   </si>
   <si>
     <t>Botão de submeter disponpivel na tela</t>
+  </si>
+  <si>
+    <t>Campo disponível e configurado para receber caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <t>Campo disponível e configurado para receber caracteres numéricos</t>
+  </si>
+  <si>
+    <t>Campo de multiplica clicável disponível</t>
+  </si>
+  <si>
+    <t>Realizado o envio de um avatar mockado através das fixtures</t>
+  </si>
+  <si>
+    <t>Editar um Heroi</t>
+  </si>
+  <si>
+    <t>Eu como usuário administrador logado, desejo editar um heroi</t>
+  </si>
+  <si>
+    <t>Clicar no botão para editar um heroi</t>
+  </si>
+  <si>
+    <t>Inserir um novo nome para o heroi</t>
+  </si>
+  <si>
+    <t>Inserir um novo preço para o heroi</t>
+  </si>
+  <si>
+    <t>Inserir uma nova quantidade de curtidas iniciais do heroi</t>
+  </si>
+  <si>
+    <t>Inserir uma nova quantidade incial de contratações do heroi</t>
+  </si>
+  <si>
+    <t>Escolher o novo poder do heroi</t>
+  </si>
+  <si>
+    <t>Escolher o novo avatar do heroi</t>
+  </si>
+  <si>
+    <t>Botão submeteu a criação, salvou as alterações e redirecionou para a página dos heróis</t>
+  </si>
+  <si>
+    <t>Botão submeteu a criação, salvou as informações e redirecionou para a página dos heróis</t>
+  </si>
+  <si>
+    <t>Deletar um heroi</t>
+  </si>
+  <si>
+    <t>Eu como usuário admnistrador logado, desejo deletar um heroi</t>
+  </si>
+  <si>
+    <t>Clicar no ícone / botão de deletar</t>
+  </si>
+  <si>
+    <t>Clicar no botão para confirmar a exclusão do heroi</t>
+  </si>
+  <si>
+    <t>Botão disponível, exibe um modal com a confirmação ou não da exclusão</t>
+  </si>
+  <si>
+    <t>Botão disponível, deleta o heroi e redireciona para a pagina de herois</t>
+  </si>
+  <si>
+    <t>Modal exibido com as infomações de confirmar ou desistir da exclusão</t>
+  </si>
+  <si>
+    <t>Excluiu o heroi e redirecionou para a página principal</t>
+  </si>
+  <si>
+    <t>Desistir da exçusão</t>
+  </si>
+  <si>
+    <t>Eu como usuário admnistrador logado, desejo desistir de deletar um heroi</t>
+  </si>
+  <si>
+    <t>Clicar no botão para cancelar a exclusão</t>
+  </si>
+  <si>
+    <t>Operação de exclusão cancelada</t>
   </si>
 </sst>
 </file>
@@ -372,7 +394,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\.m"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -394,13 +416,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -441,7 +456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,12 +467,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF434343"/>
         <bgColor rgb="FF434343"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF666666"/>
-        <bgColor rgb="FF666666"/>
       </patternFill>
     </fill>
     <fill>
@@ -491,7 +500,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -666,21 +675,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF284E3F"/>
       </left>
       <right/>
@@ -692,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -724,62 +718,97 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="49">
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="2"/>
@@ -1221,14 +1250,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="Casos de Testes Cadastro-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="44"/>
-      <tableStyleElement type="firstRowStripe" dxfId="43"/>
-      <tableStyleElement type="secondRowStripe" dxfId="42"/>
+      <tableStyleElement type="headerRow" dxfId="48"/>
+      <tableStyleElement type="firstRowStripe" dxfId="47"/>
+      <tableStyleElement type="secondRowStripe" dxfId="46"/>
     </tableStyle>
     <tableStyle name="Casos de Testes Login-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="41"/>
-      <tableStyleElement type="firstRowStripe" dxfId="40"/>
-      <tableStyleElement type="secondRowStripe" dxfId="39"/>
+      <tableStyleElement type="headerRow" dxfId="45"/>
+      <tableStyleElement type="firstRowStripe" dxfId="44"/>
+      <tableStyleElement type="secondRowStripe" dxfId="43"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1271,8 +1300,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BC73408C-81A1-48D1-8F13-6717416C4DE9}" name="Casos_de_Testes_de_Cdastro4" displayName="Casos_de_Testes_de_Cdastro4" ref="A1:E43">
-  <autoFilter ref="A1:E43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BC73408C-81A1-48D1-8F13-6717416C4DE9}" name="Casos_de_Testes_de_Cdastro4" displayName="Casos_de_Testes_de_Cdastro4" ref="A1:E46">
+  <autoFilter ref="A1:E46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{1D37A878-E798-421B-A727-C232DAE7ADF1}" name="Tarefa"/>
     <tableColumn id="2" xr3:uid="{357F3411-C044-4F9D-8E9A-D912BA9EC96D}" name="Passos"/>
@@ -1487,8 +1516,8 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1501,373 +1530,373 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
-        <v>73</v>
+      <c r="A2" s="19" t="s">
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="20">
+      <c r="A3" s="18">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>43</v>
+      <c r="B3" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
-        <v>42</v>
+      <c r="A8" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="20">
+      <c r="A9" s="18">
         <v>2</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>43</v>
+      <c r="B9" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B13" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>50</v>
+      <c r="B14" s="20" t="s">
+        <v>31</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="20">
+      <c r="A15" s="18">
         <v>3</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="D17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
+      <c r="D18" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" t="s">
-        <v>57</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>59</v>
+      <c r="A20" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="20">
-        <v>4</v>
-      </c>
-      <c r="B21" s="24" t="s">
+      <c r="A21" s="18">
+        <v>4</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
         <v>43</v>
       </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="D23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" t="s">
-        <v>57</v>
-      </c>
       <c r="D25" s="5" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
@@ -1876,21 +1905,21 @@
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="D27" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="D29" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -1898,7 +1927,7 @@
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
@@ -1912,21 +1941,21 @@
       <c r="A32" s="8"/>
       <c r="B32" s="5"/>
       <c r="D32" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="D33" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="5"/>
       <c r="D34" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -1934,7 +1963,7 @@
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
@@ -1948,21 +1977,21 @@
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="D37" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="5"/>
       <c r="D38" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="D39" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1970,23 +1999,23 @@
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
       <formula>"Bloqueado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="10" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D7 D9:D13">
-    <cfRule type="cellIs" dxfId="35" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="22" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="23">
@@ -2001,7 +2030,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D19">
-    <cfRule type="cellIs" dxfId="34" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="20" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="21">
@@ -2016,7 +2045,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -2031,7 +2060,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D25">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -2046,7 +2075,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -2061,7 +2090,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D30">
-    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="16" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="17">
@@ -2076,7 +2105,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D35">
-    <cfRule type="cellIs" dxfId="29" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="14" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="15">
@@ -2091,7 +2120,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D40">
-    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="12" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="13">
@@ -2124,9 +2153,9 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2138,255 +2167,255 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
-        <v>74</v>
+      <c r="A2" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="20">
+      <c r="A3" s="18">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>76</v>
+      <c r="B3" s="22" t="s">
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="7"/>
       <c r="D5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
       <c r="D7" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
-        <v>77</v>
+      <c r="A8" s="19" t="s">
+        <v>58</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="20">
+      <c r="A9" s="18">
         <v>2</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>79</v>
+      <c r="B9" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
-        <v>40</v>
+      <c r="A10" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="25"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="7"/>
       <c r="D11" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
       <c r="D13" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>85</v>
+      <c r="A14" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>66</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="20">
+      <c r="A15" s="18">
         <v>3</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>79</v>
+      <c r="B15" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>46</v>
+      <c r="A16" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="25"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="7"/>
       <c r="D17" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="26"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="5"/>
       <c r="D18" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
       <c r="D19" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="22"/>
       <c r="D21" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="5"/>
       <c r="D22" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="25"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="7"/>
       <c r="D23" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="26"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="5"/>
       <c r="D24" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
       <c r="D25" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
@@ -2395,21 +2424,21 @@
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="D27" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="D29" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -2417,7 +2446,7 @@
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
@@ -2431,21 +2460,21 @@
       <c r="A32" s="8"/>
       <c r="B32" s="5"/>
       <c r="D32" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="D33" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="5"/>
       <c r="D34" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -2453,7 +2482,7 @@
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
@@ -2467,21 +2496,21 @@
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="D37" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="5"/>
       <c r="D38" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="D39" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2489,23 +2518,23 @@
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="11" operator="equal">
       <formula>"Bloqueado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D7 D9:D13">
-    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="22" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="23">
@@ -2520,7 +2549,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D19">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -2533,7 +2562,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="20" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="21">
@@ -2548,7 +2577,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
@@ -2563,7 +2592,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D25">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -2576,7 +2605,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="8">
@@ -2591,7 +2620,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -2606,7 +2635,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D30">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="18" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="19">
@@ -2621,7 +2650,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D35">
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="17">
@@ -2636,7 +2665,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D40">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="15">
@@ -2667,415 +2696,596 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="74.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" customWidth="1"/>
-    <col min="5" max="5" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
-        <v>91</v>
+      <c r="A2" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="20">
+      <c r="A3" s="18">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>93</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="B11" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
-      <c r="B11" s="2"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
-      <c r="B12" s="24"/>
+      <c r="A12" s="18">
+        <v>1</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
       <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
       <c r="D13" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="E13" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>88</v>
+      </c>
       <c r="D14" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="E14" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="26"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
       <c r="D15" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
       <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
+      <c r="E16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="E18" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="23"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
       <c r="D19" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="25"/>
-      <c r="B20" s="7"/>
-      <c r="D20" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="E19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="26"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="18">
+        <v>1</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" t="s">
+        <v>111</v>
+      </c>
       <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="E21" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" t="s">
+        <v>112</v>
+      </c>
       <c r="D22" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
+      <c r="E22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="23"/>
+      <c r="B23" s="7"/>
+      <c r="D23" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="24"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="5"/>
       <c r="D24" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
       <c r="D25" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="25"/>
-      <c r="B26" s="7"/>
-      <c r="D26" s="5" t="s">
-        <v>5</v>
-      </c>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="26"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="18">
+        <v>1</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" t="s">
+        <v>111</v>
+      </c>
       <c r="D27" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="E27" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
       <c r="D28" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="21"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4"/>
+      <c r="E28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="23"/>
+      <c r="B29" s="7"/>
+      <c r="D29" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="5"/>
       <c r="D30" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="26"/>
       <c r="D31" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
-      <c r="B32" s="7"/>
-      <c r="D32" s="5" t="s">
-        <v>5</v>
-      </c>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="19"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
       <c r="D33" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="5"/>
+      <c r="D34" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
       <c r="D35" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
       <c r="D36" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="5"/>
-      <c r="D37" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="5"/>
       <c r="D38" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="4"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="D39" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="5"/>
       <c r="D40" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
       <c r="D41" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="6"/>
-      <c r="B42" s="7"/>
-      <c r="D42" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
       <c r="D43" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="8"/>
+      <c r="B44" s="5"/>
+      <c r="D44" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="D45" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="9"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>"Bloqueado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D16 D3:D10">
-    <cfRule type="cellIs" dxfId="11" priority="26" operator="equal">
+  <conditionalFormatting sqref="D21:D25 D3:D10 D12:D19">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="27">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D10">
+    <cfRule type="cellIs" dxfId="14" priority="33" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D25 D3:D10 D12:D19">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3086,11 +3296,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18:D22">
-    <cfRule type="cellIs" dxfId="10" priority="24" operator="equal">
+  <conditionalFormatting sqref="D21:D25">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3100,12 +3310,10 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="31" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3116,11 +3324,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24:D28">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+  <conditionalFormatting sqref="D10 D25 D19">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3131,38 +3339,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
-      <formula>"Pronto"</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30:D33">
-    <cfRule type="cellIs" dxfId="6" priority="22" operator="equal">
-      <formula>"Pronto"</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35:D38">
-    <cfRule type="cellIs" dxfId="5" priority="20" operator="equal">
+  <conditionalFormatting sqref="D25">
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="21">
@@ -3176,8 +3354,21 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40:D43">
-    <cfRule type="cellIs" dxfId="4" priority="18" operator="equal">
+  <conditionalFormatting sqref="D29:D31">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="19">
@@ -3191,11 +3382,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24:D28">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="7" priority="16" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3206,8 +3397,100 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18:D22 D12:D16 D3:D10">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+  <conditionalFormatting sqref="D33:D36">
+    <cfRule type="cellIs" dxfId="6" priority="29" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:D41">
+    <cfRule type="cellIs" dxfId="5" priority="27" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43:D46">
+    <cfRule type="cellIs" dxfId="4" priority="25" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D10 D12:D19">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D19">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:D28">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:D28">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:D28">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Pronto"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"Pronto"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -3221,38 +3504,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10 D22 D16">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"Pronto"</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18:D22">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Pronto"</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D35:D38 D30:D33 D40:D43 D24:D28 D18:D22 D3:D16" xr:uid="{114A343E-435B-4E65-82C9-A3F3E795374C}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D38:D41 D33:D36 D43:D46 D3:D19 D21:D25 D27:D31" xr:uid="{114A343E-435B-4E65-82C9-A3F3E795374C}">
       <formula1>"Pronto,Passou,Bloqueado,Falhou"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3264,176 +3517,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="97.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3448,28 +3531,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>25</v>
+      <c r="A1" s="11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>19</v>
+      <c r="A2" s="12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>5</v>
+      <c r="A3" s="13" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
-        <v>26</v>
+      <c r="A4" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
-        <v>27</v>
+      <c r="A5" s="15" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>